<commit_message>
identity tests for observation and deviation names
</commit_message>
<xml_diff>
--- a/input/spectrophotometry/dsl.3/data.input.xlsx
+++ b/input/spectrophotometry/dsl.3/data.input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\dsl.3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\spectrophotometry\dsl.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF58034-0961-4B08-B218-60B3CAB6858D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B4DA7F-22FC-4354-BFFE-20916ACEB8EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -1219,7 +1219,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>